<commit_message>
GFG. Stickler Thief(Maximum sum of non-adjacent elements)
GFG. Stickler Thief(Maximum sum of non-adjacent elements)
</commit_message>
<xml_diff>
--- a/Dynamic Programming/Question_List-Java version.xlsx
+++ b/Dynamic Programming/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE20C30-DF3B-4172-9D87-D0A74D63FE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B11335B-CFE1-43E5-901A-49CD62821667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Question No</t>
   </si>
@@ -58,6 +58,21 @@
   </si>
   <si>
     <t>DP(Recurrsion+Memonization+Tabulation</t>
+  </si>
+  <si>
+    <t>Stickler Thief/Maximum sum of non-adjacent elements</t>
+  </si>
+  <si>
+    <t>GFG/Coding ninja</t>
+  </si>
+  <si>
+    <t>DP(Recurrsion+Memonization+Tabulation+space optimization)</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>GFG</t>
   </si>
 </sst>
 </file>
@@ -432,7 +447,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,7 +481,9 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -483,10 +500,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>

</xml_diff>

<commit_message>
213. House Robber II
213. House Robber II-space optimization approach
</commit_message>
<xml_diff>
--- a/Dynamic Programming/Question_List-Java version.xlsx
+++ b/Dynamic Programming/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B11335B-CFE1-43E5-901A-49CD62821667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0A8E41-626F-4959-9E6B-2163E5311FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Question No</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Java</t>
   </si>
   <si>
-    <t>Coding Ninja</t>
-  </si>
-  <si>
     <t>GFG/LC/Coding Ninja</t>
   </si>
   <si>
@@ -60,12 +57,6 @@
     <t>DP(Recurrsion+Memonization+Tabulation</t>
   </si>
   <si>
-    <t>Stickler Thief/Maximum sum of non-adjacent elements</t>
-  </si>
-  <si>
-    <t>GFG/Coding ninja</t>
-  </si>
-  <si>
     <t>DP(Recurrsion+Memonization+Tabulation+space optimization)</t>
   </si>
   <si>
@@ -73,6 +64,21 @@
   </si>
   <si>
     <t>GFG</t>
+  </si>
+  <si>
+    <t>LC/CN</t>
+  </si>
+  <si>
+    <t>GFG/CN</t>
+  </si>
+  <si>
+    <t>House Robber II-Circular placement</t>
+  </si>
+  <si>
+    <t>Stickler Thief/Maximum sum of non-adjacent elements/House Robber I</t>
+  </si>
+  <si>
+    <t>DP(Space optimizatio)</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,7 +471,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -477,50 +483,62 @@
         <v>3</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>215</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
63. Unique Path II
63. Unique Path II
</commit_message>
<xml_diff>
--- a/Dynamic Programming/Question_List-Java version.xlsx
+++ b/Dynamic Programming/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC217CA-8343-4A9F-9B6C-8DF083D3E84F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8849A1A-2B07-4615-AADA-C61A3F41A20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Question No</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>https://leetcode.com/problems/unique-paths/description/</t>
+  </si>
+  <si>
+    <t>Unique Paths II</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,9 +596,24 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="1">
+        <v>63</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>

</xml_diff>

<commit_message>
64. Minimum Path Sum
64. Minimum Path Sum
</commit_message>
<xml_diff>
--- a/Dynamic Programming/Question_List-Java version.xlsx
+++ b/Dynamic Programming/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8849A1A-2B07-4615-AADA-C61A3F41A20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD3CF1D-0445-4003-B7C3-FE03A587E970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Question No</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>Unique Paths II</t>
+  </si>
+  <si>
+    <t>Minimum Path Sum</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" sqref="D8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,9 +619,21 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="1">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
CN. Maximum Path sum (recurrssion,tabulation,memoization,space optimization)
CN. Maximum Path sum (recurrssion,tabulation,memoization,space optimization)
</commit_message>
<xml_diff>
--- a/Dynamic Programming/Question_List-Java version.xlsx
+++ b/Dynamic Programming/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697027CE-9C52-44B1-9595-14E33AB86F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259F7F8-C631-4E65-B32F-54ECA8DBB2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>Question No</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Minimum Path Sum</t>
+  </si>
+  <si>
+    <t>Maximum Path Sum in the matrix</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:E8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +486,7 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="70.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" style="10" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" style="10" customWidth="1"/>
     <col min="6" max="6" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -635,10 +638,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="D9" s="6"/>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
931. Minimum Falling Path Sum (recurrssion, tabulation, memiozation)
931. Minimum Falling Path Sum (recurrssion, tabulation, memiozation)
</commit_message>
<xml_diff>
--- a/Dynamic Programming/Question_List-Java version.xlsx
+++ b/Dynamic Programming/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259F7F8-C631-4E65-B32F-54ECA8DBB2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F20A15-10DA-4C6C-B8DF-1219945472BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Question No</t>
   </si>
@@ -106,13 +106,16 @@
   </si>
   <si>
     <t>Maximum Path Sum in the matrix</t>
+  </si>
+  <si>
+    <t>Minimum Falling Path Sum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +131,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -138,7 +156,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,17 +173,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -175,14 +187,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -194,6 +200,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,36 +500,36 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="70.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="48.28515625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="48.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="16" customFormat="1" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -523,7 +546,7 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
@@ -543,7 +566,7 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -560,7 +583,7 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -577,27 +600,27 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -608,16 +631,16 @@
       <c r="B7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -631,182 +654,191 @@
       <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:6" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="D10" s="6"/>
+    <row r="10" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>931</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
-      <c r="D11" s="6"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
+      <c r="A12" s="2"/>
       <c r="B12" s="1"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="8"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="11"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="8"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
-      <c r="C33" s="5"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
-      <c r="C34" s="5"/>
+      <c r="C34" s="3"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
-      <c r="C35" s="5"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="1"/>
-      <c r="C36" s="5"/>
+      <c r="C36" s="3"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1"/>
-      <c r="C37" s="5"/>
+      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="1"/>

</xml_diff>

<commit_message>
Coding ninja. Chocalate pickup
Coding ninja. Chocalate pickup
</commit_message>
<xml_diff>
--- a/Dynamic Programming/Question_List-Java version.xlsx
+++ b/Dynamic Programming/Question_List-Java version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Dynamic Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016CC289-C6E0-4EEA-B2E3-F02CD3C7B8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CECE052-6C76-42B5-836D-C2EB95601B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Question No</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>Minimum Falling Path Sum</t>
+  </si>
+  <si>
+    <t>Chocolate Pickup</t>
+  </si>
+  <si>
+    <t>Recurrssion</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,8 +702,21 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>

</xml_diff>